<commit_message>
updated the pcr rack def files
</commit_message>
<xml_diff>
--- a/cherrypick/cherrypick_example.xlsx
+++ b/cherrypick/cherrypick_example.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikpoppleton/software/opentrons/cherrypick/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2501A0-88E8-4C4D-8CFB-106FD25E798B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AB6605-AFCA-B64C-B85F-AFDE569A6CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{ACB8BC66-A036-5949-B257-88360FBD43E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,7 +461,8 @@
         <v>7</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <f>5*5</f>
+        <v>25</v>
       </c>
       <c r="G2">
         <v>1</v>

</xml_diff>